<commit_message>
Aggiunta di controllo e installazione automatica dei pacchetti necessari in progetto.R
</commit_message>
<xml_diff>
--- a/results/Risultati.xlsx
+++ b/results/Risultati.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t xml:space="preserve">Linguaggio</t>
   </si>
@@ -28,7 +28,76 @@
     <t xml:space="preserve">Risultato (MCC)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tempo d’esecuzione (s)</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tempo 1</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">a</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> esecuzione (s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tempo 2</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">a</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> esecuzione (s)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Python</t>
@@ -75,7 +144,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -100,6 +169,15 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <vertAlign val="superscript"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -175,21 +253,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -442,81 +528,90 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="31.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="31.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>